<commit_message>
Add multiple choice field to questions.
</commit_message>
<xml_diff>
--- a/Documentation/Files from client/Data Fields 20160928.xlsx
+++ b/Documentation/Files from client/Data Fields 20160928.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="DataItems" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -606,6 +612,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,9 +924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1551,7 +1560,7 @@
       <c r="A44" s="4">
         <v>37</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -1568,7 +1577,7 @@
       <c r="A45" s="6">
         <v>38</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1585,7 +1594,7 @@
       <c r="A46" s="6">
         <v>39</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -1602,7 +1611,7 @@
       <c r="A47" s="6">
         <v>40</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -1619,7 +1628,7 @@
       <c r="A48" s="6">
         <v>41</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -1636,7 +1645,7 @@
       <c r="A49" s="6">
         <v>42</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -1653,7 +1662,7 @@
       <c r="A50" s="6">
         <v>43</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -1670,7 +1679,7 @@
       <c r="A51" s="6">
         <v>44</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -1687,7 +1696,7 @@
       <c r="A52" s="6">
         <v>45</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -1704,7 +1713,7 @@
       <c r="A53" s="6">
         <v>46</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -1721,7 +1730,7 @@
       <c r="A54" s="6">
         <v>47</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -1738,7 +1747,7 @@
       <c r="A55" s="6">
         <v>48</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -1755,7 +1764,7 @@
       <c r="A56" s="6">
         <v>49</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -1772,7 +1781,7 @@
       <c r="A57" s="6">
         <v>50</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -1789,7 +1798,7 @@
       <c r="A58" s="6">
         <v>51</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -1806,7 +1815,7 @@
       <c r="A59" s="4">
         <v>52</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -1823,7 +1832,7 @@
       <c r="A60" s="4">
         <v>53</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -1840,7 +1849,7 @@
       <c r="A61" s="4">
         <v>54</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -1857,7 +1866,7 @@
       <c r="A62" s="4">
         <v>55</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C62" s="4" t="s">

</xml_diff>